<commit_message>
Excel files and Testfile Bug done Commit
</commit_message>
<xml_diff>
--- a/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
+++ b/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IntelljWorkspaces\src\main\java\com\denovo\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D9C48-60EF-4F91-BE01-7C93E3611914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B958A462-4F26-4B6F-AA18-AA7F00332722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="12" activeTab="16" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="1" activeTab="4" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="iso(Primary)MerchantWithFee" sheetId="12" r:id="rId2"/>
+    <sheet name="Iso(Primary)MerchantWithFee" sheetId="12" r:id="rId2"/>
     <sheet name="ISO(Primary)MerchantWithoutFee" sheetId="16" r:id="rId3"/>
     <sheet name="ISO(Addon)MerchantWithFee" sheetId="17" r:id="rId4"/>
     <sheet name="ISO(Addon)AddMerchantWithoutFee" sheetId="18" r:id="rId5"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="96">
   <si>
     <t>USERNAME</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>Select Profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MID</t>
   </si>
   <si>
     <t>Agent</t>
@@ -897,16 +894,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>6</v>
@@ -957,48 +954,48 @@
         <v>25</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>13</v>
@@ -1007,10 +1004,10 @@
         <v>14</v>
       </c>
       <c r="K2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>90</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>17</v>
@@ -1019,40 +1016,40 @@
         <v>17</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="S2" s="14" t="s">
+      <c r="T2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1106,16 +1103,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>6</v>
@@ -1166,48 +1163,48 @@
         <v>25</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>13</v>
@@ -1216,10 +1213,10 @@
         <v>14</v>
       </c>
       <c r="K2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>90</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>17</v>
@@ -1228,40 +1225,40 @@
         <v>17</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="S2" s="14" t="s">
+      <c r="T2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1312,16 +1309,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>6</v>
@@ -1372,48 +1369,48 @@
         <v>25</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>13</v>
@@ -1422,10 +1419,10 @@
         <v>14</v>
       </c>
       <c r="K2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>90</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>17</v>
@@ -1434,40 +1431,40 @@
         <v>17</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="S2" s="14" t="s">
+      <c r="T2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1514,16 +1511,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>6</v>
@@ -1574,48 +1571,48 @@
         <v>25</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>13</v>
@@ -1624,10 +1621,10 @@
         <v>14</v>
       </c>
       <c r="K2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>90</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>17</v>
@@ -1636,40 +1633,40 @@
         <v>17</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="S2" s="14" t="s">
+      <c r="T2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1714,16 +1711,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>16</v>
@@ -1750,36 +1747,36 @@
         <v>25</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1788,40 +1785,40 @@
         <v>17</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1855,16 +1852,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>16</v>
@@ -1891,36 +1888,36 @@
         <v>25</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -1929,40 +1926,40 @@
         <v>17</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1998,16 +1995,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>16</v>
@@ -2034,36 +2031,36 @@
         <v>25</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
         <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -2072,40 +2069,40 @@
         <v>17</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2121,7 +2118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC00A5E-BBFA-4D51-A5A5-260E3569093C}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
@@ -2139,16 +2136,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>16</v>
@@ -2175,36 +2172,36 @@
         <v>25</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
         <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
@@ -2213,40 +2210,40 @@
         <v>17</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2262,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2E5959-08A6-4DD3-802A-D5662CFE3B61}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2297,10 +2294,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -2330,10 +2327,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>16</v>
@@ -2360,63 +2357,63 @@
         <v>25</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>17</v>
@@ -2425,40 +2422,40 @@
         <v>17</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="V2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2477,8 +2474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD378E3F-B89B-440E-9DFC-E4DE5C82F17D}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2514,10 +2511,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -2547,10 +2544,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>16</v>
@@ -2577,63 +2574,63 @@
         <v>25</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="I2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>17</v>
@@ -2642,40 +2639,40 @@
         <v>17</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="U2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2695,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0199BBB-85E2-4252-BC39-A69F2965ADDE}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2711,10 +2708,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -2744,10 +2741,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>16</v>
@@ -2774,61 +2771,61 @@
         <v>25</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>58</v>
-      </c>
       <c r="G2" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>17</v>
@@ -2837,40 +2834,40 @@
         <v>17</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="14" t="s">
+      <c r="U2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2888,8 +2885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A077435-D7EB-484D-8D4C-8825BE253336}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2917,10 +2914,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -2950,10 +2947,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>16</v>
@@ -2980,63 +2977,63 @@
         <v>25</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>17</v>
@@ -3045,40 +3042,40 @@
         <v>17</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="U2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3131,10 +3128,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -3164,10 +3161,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>16</v>
@@ -3194,63 +3191,63 @@
         <v>25</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>17</v>
@@ -3259,40 +3256,40 @@
         <v>17</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="14" t="s">
+      <c r="U2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3333,10 +3330,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -3366,10 +3363,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>16</v>
@@ -3396,63 +3393,63 @@
         <v>25</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>17</v>
@@ -3461,40 +3458,40 @@
         <v>17</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="U2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3537,10 +3534,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -3570,10 +3567,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>16</v>
@@ -3600,63 +3597,63 @@
         <v>25</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>17</v>
@@ -3665,40 +3662,40 @@
         <v>17</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="14" t="s">
+      <c r="U2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3748,10 +3745,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -3781,10 +3778,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>16</v>
@@ -3811,63 +3808,63 @@
         <v>25</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>17</v>
@@ -3876,40 +3873,40 @@
         <v>17</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="U2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
existing All file changes, removed unused page and testscript
</commit_message>
<xml_diff>
--- a/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
+++ b/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IntelljWorkspaces\src\main\java\com\denovo\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DenovoPortal Automation Monitoring System\src\main\java\com\denovo\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ECBF2E-AC8B-48CD-BF7F-EB271A31BEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B86B90D-6FFF-4667-8575-BFB4215756CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="13" activeTab="18" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="825" firstSheet="13" activeTab="18" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,8 @@
     <sheet name="AgentOffice(P)AddTpn" sheetId="27" r:id="rId16"/>
     <sheet name="AgentOffice(A)AddTpn" sheetId="28" r:id="rId17"/>
     <sheet name="SystemLoginDashboard" sheetId="29" r:id="rId18"/>
-    <sheet name="SystemLoginTransaction" sheetId="30" r:id="rId19"/>
+    <sheet name="IsoLoginDashboard" sheetId="31" r:id="rId19"/>
+    <sheet name="SystemLoginTransaction" sheetId="30" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="102">
   <si>
     <t>USERNAME</t>
   </si>
@@ -350,6 +351,9 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>ISOPrimaryPWD</t>
   </si>
 </sst>
 </file>
@@ -2290,7 +2294,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2332,25 +2336,26 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FF51A8-1278-47BF-B39F-EB761BD58E51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B261820-8774-4728-8342-FA5627569B01}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" customWidth="1"/>
-    <col min="2" max="2" width="39.7265625" customWidth="1"/>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>98</v>
@@ -2364,13 +2369,13 @@
         <v>61</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D995C19C-73E5-4D94-9CFC-E9F7E5BB06EE}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{DD527FF8-7316-4F3A-863E-FA7EC134E824}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B696F878-68BE-4A0F-850D-67EDB267A5A6}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{DFD8D6F5-0E95-43A1-BFC0-DA293B4BDB1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2588,6 +2593,51 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FF51A8-1278-47BF-B39F-EB761BD58E51}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="39.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D995C19C-73E5-4D94-9CFC-E9F7E5BB06EE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{DD527FF8-7316-4F3A-863E-FA7EC134E824}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ISO Transaction page added
</commit_message>
<xml_diff>
--- a/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
+++ b/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DenovoPortal Automation Monitoring System\src\main\java\com\denovo\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B86B90D-6FFF-4667-8575-BFB4215756CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6392EBB-CFCC-48FA-A5B6-98B5C0D9890F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="825" firstSheet="13" activeTab="18" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="16" activeTab="20" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="SystemLoginDashboard" sheetId="29" r:id="rId18"/>
     <sheet name="IsoLoginDashboard" sheetId="31" r:id="rId19"/>
     <sheet name="SystemLoginTransaction" sheetId="30" r:id="rId20"/>
+    <sheet name="IsoLoginTransaction" sheetId="32" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="103">
   <si>
     <t>USERNAME</t>
   </si>
@@ -354,6 +355,9 @@
   </si>
   <si>
     <t>ISOPrimaryPWD</t>
+  </si>
+  <si>
+    <t>suknecosti@vusra.com</t>
   </si>
 </sst>
 </file>
@@ -2339,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B261820-8774-4728-8342-FA5627569B01}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2363,7 +2367,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>61</v>
@@ -2374,8 +2378,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B696F878-68BE-4A0F-850D-67EDB267A5A6}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{DFD8D6F5-0E95-43A1-BFC0-DA293B4BDB1E}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DFD8D6F5-0E95-43A1-BFC0-DA293B4BDB1E}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{539C05B2-CFA6-465E-B41C-D9E23910CCBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2600,7 +2604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FF51A8-1278-47BF-B39F-EB761BD58E51}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2608,6 +2612,7 @@
   <cols>
     <col min="1" max="1" width="29.1796875" customWidth="1"/>
     <col min="2" max="2" width="39.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
@@ -2636,6 +2641,52 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D995C19C-73E5-4D94-9CFC-E9F7E5BB06EE}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{DD527FF8-7316-4F3A-863E-FA7EC134E824}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C57487-1B7E-4B61-ABD8-D1204A496E09}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.7265625" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4C5F86C1-1388-4B8C-B27C-71B0E3F68977}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{70A515F0-FCDB-417E-A673-D32C2D739EAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DriverFactory, edge,safari browser added
</commit_message>
<xml_diff>
--- a/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
+++ b/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DenovoPortal Automation Monitoring System\src\main\java\com\denovo\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IPOSPAYS-Automation-Monitoring-System\src\main\java\com\denovo\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6392EBB-CFCC-48FA-A5B6-98B5C0D9890F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98F5227-751F-42E6-ABAB-DD31C0B4D867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="16" activeTab="20" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="16" activeTab="17" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="104">
   <si>
     <t>USERNAME</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>suknecosti@vusra.com</t>
+  </si>
+  <si>
+    <t>safari</t>
   </si>
 </sst>
 </file>
@@ -2295,10 +2298,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D57-EF3B-450C-BCDA-635CAD1C69EA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2330,10 +2333,23 @@
         <v>100</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6498C75C-7BF4-42B2-8F17-9AAD08DF9A4D}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4C49319C-DB9A-40A5-9E7D-FA6084AD9004}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{E5708D5C-FBF7-4EFD-B312-EAC1F4DBF8FF}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{6E4633AE-5139-4A43-8B1D-AAC7984396FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2341,10 +2357,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B261820-8774-4728-8342-FA5627569B01}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2376,10 +2392,23 @@
         <v>100</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DFD8D6F5-0E95-43A1-BFC0-DA293B4BDB1E}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{539C05B2-CFA6-465E-B41C-D9E23910CCBB}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{65D10483-A452-4066-A90B-B9763921F017}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{7B0348BC-8246-4B46-A5CA-0D8B0561F2F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2602,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FF51A8-1278-47BF-B39F-EB761BD58E51}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2637,10 +2666,23 @@
         <v>99</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D995C19C-73E5-4D94-9CFC-E9F7E5BB06EE}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{DD527FF8-7316-4F3A-863E-FA7EC134E824}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{8461F8E8-F76D-4554-BB2D-70605F40DD66}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{7F2B3614-108B-45A6-A23F-18EA16D9FB55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2648,10 +2690,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C57487-1B7E-4B61-ABD8-D1204A496E09}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2683,10 +2725,23 @@
         <v>99</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{4C5F86C1-1388-4B8C-B27C-71B0E3F68977}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{70A515F0-FCDB-417E-A673-D32C2D739EAF}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{D46CFA31-2524-4C57-9F40-475DF0B22D67}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{0FB8AE65-6A07-4BAD-91ED-B2165BF3E791}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
xml file,change thread to 1
</commit_message>
<xml_diff>
--- a/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
+++ b/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IPOSPAYS-Automation-Monitoring-System\src\main\java\com\denovo\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98F5227-751F-42E6-ABAB-DD31C0B4D867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C1733E-3DAD-49EC-BD42-4C45A2FDC3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="16" activeTab="17" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="16" activeTab="20" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="103">
   <si>
     <t>USERNAME</t>
   </si>
@@ -358,9 +358,6 @@
   </si>
   <si>
     <t>suknecosti@vusra.com</t>
-  </si>
-  <si>
-    <t>safari</t>
   </si>
 </sst>
 </file>
@@ -2300,7 +2297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D57-EF3B-450C-BCDA-635CAD1C69EA}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2341,7 +2338,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2400,7 +2397,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2634,7 +2631,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2674,7 +2671,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2692,7 +2689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C57487-1B7E-4B61-ABD8-D1204A496E09}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2733,7 +2730,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New merchantpage and Test page added
</commit_message>
<xml_diff>
--- a/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
+++ b/src/main/java/com/denovo/ExcelData/SE_DataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IPOSPAYS-Automation-Monitoring-System\src\main\java\com\denovo\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158561E6-D992-41CA-BBE5-5075257FBA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599556CB-9387-4436-8F0B-5605B89B5508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="16" activeTab="17" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="825" firstSheet="16" activeTab="19" xr2:uid="{7F7405CC-6F03-4509-8AFD-A92E532AE18E}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,10 @@
     <sheet name="AgentOffice(P)AddTpn" sheetId="27" r:id="rId16"/>
     <sheet name="AgentOffice(A)AddTpn" sheetId="28" r:id="rId17"/>
     <sheet name="SystemLoginDashboard" sheetId="29" r:id="rId18"/>
-    <sheet name="IsoLoginDashboard" sheetId="31" r:id="rId19"/>
-    <sheet name="SystemLoginTransaction" sheetId="30" r:id="rId20"/>
-    <sheet name="IsoLoginTransaction" sheetId="32" r:id="rId21"/>
+    <sheet name="SystemLoginMerchant" sheetId="33" r:id="rId19"/>
+    <sheet name="IsoLoginDashboard" sheetId="31" r:id="rId20"/>
+    <sheet name="SystemLoginTransaction" sheetId="30" r:id="rId21"/>
+    <sheet name="IsoLoginTransaction" sheetId="32" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="104">
   <si>
     <t>USERNAME</t>
   </si>
@@ -2300,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD237D57-EF3B-450C-BCDA-635CAD1C69EA}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2356,26 +2357,26 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B261820-8774-4728-8342-FA5627569B01}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36FD959-4446-4EB0-8D72-1B0206E52EDC}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>98</v>
@@ -2383,7 +2384,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>61</v>
@@ -2394,7 +2395,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>61</v>
@@ -2405,10 +2406,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DFD8D6F5-0E95-43A1-BFC0-DA293B4BDB1E}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{539C05B2-CFA6-465E-B41C-D9E23910CCBB}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{65D10483-A452-4066-A90B-B9763921F017}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{7B0348BC-8246-4B46-A5CA-0D8B0561F2F5}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AB6769B7-656D-4D1D-8728-D3377287F645}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{B10273FD-D193-4695-B95B-6D1A2C4C9D0D}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{798DC085-4905-4D58-889A-BDB4CD64C5CD}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{10C7C658-EF0E-42C3-ADB4-78A3F6163179}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2630,6 +2631,65 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B261820-8774-4728-8342-FA5627569B01}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DFD8D6F5-0E95-43A1-BFC0-DA293B4BDB1E}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{539C05B2-CFA6-465E-B41C-D9E23910CCBB}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{65D10483-A452-4066-A90B-B9763921F017}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{7B0348BC-8246-4B46-A5CA-0D8B0561F2F5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FF51A8-1278-47BF-B39F-EB761BD58E51}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2688,7 +2748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C57487-1B7E-4B61-ABD8-D1204A496E09}">
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>